<commit_message>
fix autofence unit test - data table didn't include a key column
</commit_message>
<xml_diff>
--- a/doc/examples/operation/operation-autofence.xlsx
+++ b/doc/examples/operation/operation-autofence.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community\doc\user-guide\cookbook\operation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community\doc\examples\operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E386F1EE-2EA3-4409-867F-3D6AED88D291}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10103" tabRatio="875" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="975" yWindow="-14940" windowWidth="17280" windowHeight="9075" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sales order" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">operation!$A:$H</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'operation material'!$A:$D</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">parameter!$A:$C</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'purchase order'!$B:$G</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'purchase order'!$A$1:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sales order'!$A:$H</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">supplier!$A:$A</definedName>
   </definedNames>
@@ -168,7 +169,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
@@ -520,22 +521,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -587,7 +588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -614,27 +615,27 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1048576"/>
+  <autoFilter ref="A1:H1048576" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -656,7 +657,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -668,117 +669,117 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1048516"/>
+  <autoFilter ref="A1:C1048516" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576"/>
+  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576"/>
+  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576"/>
+  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -801,7 +802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -824,7 +825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -848,48 +849,48 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G1048576"/>
+  <autoFilter ref="A1:G3" xr:uid="{EFFA73A4-3AB4-498B-A7FB-7C92DF7BE214}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:M1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576"/>
+  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:M1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -909,7 +910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -929,7 +930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -950,22 +951,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1048576"/>
+  <autoFilter ref="A1:F1048576" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:M1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +992,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>604800</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1038,27 +1039,27 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1048576"/>
+  <autoFilter ref="A1:H1048576" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1101,7 +1102,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1048576"/>
+  <autoFilter ref="A1:D1048576" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>